<commit_message>
Add insert SQL lines
</commit_message>
<xml_diff>
--- a/backend/database/PostgreSQL-contracts.xlsx
+++ b/backend/database/PostgreSQL-contracts.xlsx
@@ -897,7 +897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
@@ -907,46 +907,46 @@
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="str">
-        <f>CONCATENATE("INSERT INTO ",'create-contracts'!$B$1," VALUES (","'",raw!A2,"', ","'",raw!B2,"', ",raw!C2,", ","'",raw!D2,"', ","'",raw!E2,"', ","'",raw!F2,"', ","'",raw!G2,"');")</f>
-        <v>INSERT INTO contracts VALUES ('CT-2016-0134', '2016-09-23', null, '2016-09-23', 'Contrato de Compra de Energia Regulada - CCER - entre o SENADO FEDERAL e a CEB Distribuição S/A, de energia elétrica para as unidades consumidoras de identificação nº 466.453-1; 491.042-7; 491.747-2; 491.750-2; 493.169-6; 605.120-0; 623.849-1; 675.051-6; 966.027-5 e 1.089.425-X.', 'CEB Distribuição S.A.', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/3842');</v>
+        <f>CONCATENATE("insert into ",'create-contracts'!$B$1," values (","'",raw!A2,"', ","'",raw!B2,"', ",raw!C2,", ","'",raw!D2,"', ","'",raw!E2,"', ","'",raw!F2,"', ","'",raw!G2,"');")</f>
+        <v>insert into contracts values ('CT-2016-0134', '2016-09-23', null, '2016-09-23', 'Contrato de Compra de Energia Regulada - CCER - entre o SENADO FEDERAL e a CEB Distribuição S/A, de energia elétrica para as unidades consumidoras de identificação nº 466.453-1; 491.042-7; 491.747-2; 491.750-2; 493.169-6; 605.120-0; 623.849-1; 675.051-6; 966.027-5 e 1.089.425-X.', 'CEB Distribuição S.A.', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/3842');</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="str">
-        <f>CONCATENATE("INSERT INTO ",'create-contracts'!$B$1," VALUES (","'",raw!A3,"', ","'",raw!B3,"', ",raw!C3,", ","'",raw!D3,"', ","'",raw!E3,"', ","'",raw!F3,"', ","'",raw!G3,"');")</f>
-        <v>INSERT INTO contracts VALUES ('CTA-2017-0119', '2017-12-29', null, '2017-12-29', 'Estabelecer as principais condições da prestação e utilização do serviço público de energia elétrica entre a CEB Distribuição S.A e o SENADO FEDERAL, de acordo com as condições gerais de fornecimento de energia elétrica e demais regulamentos expedidos pela Agência Nacional de Energia Elétrica - ANEEL - no fornecimento continuado de energia elétrica para as diversas Unidades Consumidoras do Senado Federal, durante o período de 60 (sessenta) meses consecutivos.', 'CEB Distribuição S.A.', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/4306');</v>
+        <f>CONCATENATE("insert into ",'create-contracts'!$B$1," values (","'",raw!A3,"', ","'",raw!B3,"', ",raw!C3,", ","'",raw!D3,"', ","'",raw!E3,"', ","'",raw!F3,"', ","'",raw!G3,"');")</f>
+        <v>insert into contracts values ('CTA-2017-0119', '2017-12-29', null, '2017-12-29', 'Estabelecer as principais condições da prestação e utilização do serviço público de energia elétrica entre a CEB Distribuição S.A e o SENADO FEDERAL, de acordo com as condições gerais de fornecimento de energia elétrica e demais regulamentos expedidos pela Agência Nacional de Energia Elétrica - ANEEL - no fornecimento continuado de energia elétrica para as diversas Unidades Consumidoras do Senado Federal, durante o período de 60 (sessenta) meses consecutivos.', 'CEB Distribuição S.A.', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/4306');</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="str">
-        <f>CONCATENATE("INSERT INTO ",'create-contracts'!$B$1," VALUES (","'",raw!A4,"', ","'",raw!B4,"', ",raw!C4,", ","'",raw!D4,"', ","'",raw!E4,"', ","'",raw!F4,"', ","'",raw!G4,"');")</f>
-        <v>INSERT INTO contracts VALUES ('TE-2017-0014', '2017-11-23', null, '2017-11-23', 'O Ministério de Estado do Planejamento, Desenvolvimento e Gestão, através da Secretaria de Patrimônio da União - MPDG/SPU - e a Presidência do SENADO FEDERAL, no uso de suas atribuições legais, resolvem celebrar a transferência ao Senado Federal, por meio de cessão de uso, do imóvel de propriedade da União situado no Setor de Clubes Esportivos Sul - SCE/SUL - Trecho 3 - Lote 07 - Brasília - Distrito Federal.', 'N/A', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/4262');</v>
+        <f>CONCATENATE("insert into ",'create-contracts'!$B$1," values (","'",raw!A4,"', ","'",raw!B4,"', ",raw!C4,", ","'",raw!D4,"', ","'",raw!E4,"', ","'",raw!F4,"', ","'",raw!G4,"');")</f>
+        <v>insert into contracts values ('TE-2017-0014', '2017-11-23', null, '2017-11-23', 'O Ministério de Estado do Planejamento, Desenvolvimento e Gestão, através da Secretaria de Patrimônio da União - MPDG/SPU - e a Presidência do SENADO FEDERAL, no uso de suas atribuições legais, resolvem celebrar a transferência ao Senado Federal, por meio de cessão de uso, do imóvel de propriedade da União situado no Setor de Clubes Esportivos Sul - SCE/SUL - Trecho 3 - Lote 07 - Brasília - Distrito Federal.', 'N/A', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/4262');</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="str">
-        <f>CONCATENATE("INSERT INTO ",'create-contracts'!$B$1," VALUES (","'",raw!A5,"', ","'",raw!B5,"', ",raw!C5,", ","'",raw!D5,"', ","'",raw!E5,"', ","'",raw!F5,"', ","'",raw!G5,"');")</f>
-        <v>INSERT INTO contracts VALUES ('CT-2016-0165', '2016-12-19', null, '2016-12-19', 'Contratação de empresa prestadora, de forma contínua, dos serviços públicos de abastecimento de água e esgotamento sanitário, a serem utilizados no Complexo Arquitetônico do SENADO FEDERAL pela Companhia de Saneamento Ambiental do Distrito Federal - CAESB - durante o período indeterminado de vigência contratual.', 'CAESB - Companhia de Saneamento Ambiental do Distrito Federal', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/3931');</v>
+        <f>CONCATENATE("insert into ",'create-contracts'!$B$1," values (","'",raw!A5,"', ","'",raw!B5,"', ",raw!C5,", ","'",raw!D5,"', ","'",raw!E5,"', ","'",raw!F5,"', ","'",raw!G5,"');")</f>
+        <v>insert into contracts values ('CT-2016-0165', '2016-12-19', null, '2016-12-19', 'Contratação de empresa prestadora, de forma contínua, dos serviços públicos de abastecimento de água e esgotamento sanitário, a serem utilizados no Complexo Arquitetônico do SENADO FEDERAL pela Companhia de Saneamento Ambiental do Distrito Federal - CAESB - durante o período indeterminado de vigência contratual.', 'CAESB - Companhia de Saneamento Ambiental do Distrito Federal', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/3931');</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
-        <f>CONCATENATE("INSERT INTO ",'create-contracts'!$B$1," VALUES (","'",raw!A6,"', ","'",raw!B6,"', ",raw!C6,", ","'",raw!D6,"', ","'",raw!E6,"', ","'",raw!F6,"', ","'",raw!G6,"');")</f>
-        <v>INSERT INTO contracts VALUES ('CT-2014-0088', '2014-12-09', '2019-12-08', '2014-12-09', 'Contratação de empresa especializada para a prestação de serviços de manutenção no Sistema de Geração de Energia Elétrica de Emergência, do Complexo Arquitetônico do SENADO FEDERAL, composto de 05 (cinco) grupos motores-geradores, movidos à óleo diesel, durante o período de 36 (trinta e seis) meses consecutivos.', 'RCS Tecnologia Ltda.', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/3095');</v>
+        <f>CONCATENATE("insert into ",'create-contracts'!$B$1," values (","'",raw!A6,"', ","'",raw!B6,"', ",raw!C6,", ","'",raw!D6,"', ","'",raw!E6,"', ","'",raw!F6,"', ","'",raw!G6,"');")</f>
+        <v>insert into contracts values ('CT-2014-0088', '2014-12-09', '2019-12-08', '2014-12-09', 'Contratação de empresa especializada para a prestação de serviços de manutenção no Sistema de Geração de Energia Elétrica de Emergência, do Complexo Arquitetônico do SENADO FEDERAL, composto de 05 (cinco) grupos motores-geradores, movidos à óleo diesel, durante o período de 36 (trinta e seis) meses consecutivos.', 'RCS Tecnologia Ltda.', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/3095');</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
-        <f>CONCATENATE("INSERT INTO ",'create-contracts'!$B$1," VALUES (","'",raw!A7,"', ","'",raw!B7,"', ",raw!C7,", ","'",raw!D7,"', ","'",raw!E7,"', ","'",raw!F7,"', ","'",raw!G7,"');")</f>
-        <v>INSERT INTO contracts VALUES ('CT-2016-110', '2016-08-25', '2021-08-24', '2016-08-25', 'Contratação de empresa especializada para a prestação de serviços continuados e sob demanda, referentes à operação e manutenção preventiva e corretiva do Sistema Elétrico do Complexo Arquitetônico do SENADO FEDERAL, com operação de sistema informatizado de gerenciamento de manutenção e suprimento de insumos necessários à execução dos serviços, durante o período de 36 (trinta e seis) meses consecutivos.', 'RCS Tecnologia Ltda.', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/3769');</v>
+        <f>CONCATENATE("insert into ",'create-contracts'!$B$1," values (","'",raw!A7,"', ","'",raw!B7,"', ",raw!C7,", ","'",raw!D7,"', ","'",raw!E7,"', ","'",raw!F7,"', ","'",raw!G7,"');")</f>
+        <v>insert into contracts values ('CT-2016-110', '2016-08-25', '2021-08-24', '2016-08-25', 'Contratação de empresa especializada para a prestação de serviços continuados e sob demanda, referentes à operação e manutenção preventiva e corretiva do Sistema Elétrico do Complexo Arquitetônico do SENADO FEDERAL, com operação de sistema informatizado de gerenciamento de manutenção e suprimento de insumos necessários à execução dos serviços, durante o período de 36 (trinta e seis) meses consecutivos.', 'RCS Tecnologia Ltda.', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/3769');</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
-        <f>CONCATENATE("INSERT INTO ",'create-contracts'!$B$1," VALUES (","'",raw!A8,"', ","'",raw!B8,"', ",raw!C8,", ","'",raw!D8,"', ","'",raw!E8,"', ","'",raw!F8,"', ","'",raw!G8,"');")</f>
-        <v>INSERT INTO contracts VALUES ('CT-2017-0084', '2017-10-24', '2017-12-01', '2020-11-30', 'Contratação de empresa especializada para prestação de serviços continuados e sob demanda, referentes à operação, manutenção preventiva e corretiva do Sistema Hidrossanitário em todo o Complexo Arquitetônico do SENADO FEDERAL, incluindo a operação de sistema de controle de manutenção informatizado, fornecimento de suprimentos, insumos e de mão de obra necessários à plena execução dos serviços, durante o período de 36 (trinta e seis) meses consecutivos.', 'RCS Tecnologia Ltda.', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/4298');</v>
+        <f>CONCATENATE("insert into ",'create-contracts'!$B$1," values (","'",raw!A8,"', ","'",raw!B8,"', ",raw!C8,", ","'",raw!D8,"', ","'",raw!E8,"', ","'",raw!F8,"', ","'",raw!G8,"');")</f>
+        <v>insert into contracts values ('CT-2017-0084', '2017-10-24', '2017-12-01', '2020-11-30', 'Contratação de empresa especializada para prestação de serviços continuados e sob demanda, referentes à operação, manutenção preventiva e corretiva do Sistema Hidrossanitário em todo o Complexo Arquitetônico do SENADO FEDERAL, incluindo a operação de sistema de controle de manutenção informatizado, fornecimento de suprimentos, insumos e de mão de obra necessários à plena execução dos serviços, durante o período de 36 (trinta e seis) meses consecutivos.', 'RCS Tecnologia Ltda.', 'https://www6g.senado.gov.br/transparencia/licitacoes-e-contratos/contratos/4298');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>